<commit_message>
Small adjustments from data load
</commit_message>
<xml_diff>
--- a/OpsAndMats/8027098.xlsx
+++ b/OpsAndMats/8027098.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclark.LABTESTING\Documents\ERP Notes\Phase2_BOM\OpsAndMats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC10CA33-47C6-45F0-A547-7ECDBBF3A176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Operations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -443,8 +449,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,12 +467,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -496,17 +508,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -553,7 +574,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,9 +606,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -619,6 +658,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -794,14 +851,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,256 +991,256 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
-      <c r="A2" t="s">
+    <row r="2" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>0</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
-      <c r="A3" t="s">
+    <row r="3" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
-      <c r="A4" t="s">
+    <row r="4" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>1</v>
-      </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1264,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1347,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1430,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1513,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1596,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1679,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1762,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1845,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1928,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2011,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2094,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2177,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2260,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2343,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2432,14 +2491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2647,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -2698,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -2808,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2918,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3028,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3138,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -3248,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -3358,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -3468,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -3578,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -3688,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3798,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>

</xml_diff>